<commit_message>
fixed datum/opmerkingen bug when you do not pass them
</commit_message>
<xml_diff>
--- a/data/accesskarteringinfo.xlsx
+++ b/data/accesskarteringinfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jordydelange\git\veg2hab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE631FE-BED2-44C8-82DD-F6ABD2455113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D7D3D4-BA03-44EF-9627-20A6812BBF59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17580" yWindow="2745" windowWidth="21135" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1275" yWindow="780" windowWidth="20685" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -204,75 +204,6 @@
     <t>./GR/SGL Zuidlaardermeer 2019/kartering zuidlaardermeer 2019 definitief/GIS-bestanden Zuidlaardermeer 2019/GIS_Vlakken_zuidlaardermeer_2019/vlakken.shp</t>
   </si>
   <si>
-    <t>./FR Extra/Tjonger_2021_SBB/Database/Tjonger_2021</t>
-  </si>
-  <si>
-    <t>./FR Extra/Witte en zwarte brekken Veg&amp;Flora 2021/turbovegDS/Wite_en_Swarte_Brekken_2021</t>
-  </si>
-  <si>
-    <t>./DR Extra/definitief Fochteloo_Norg2020/DS_NM_SBB v3.0Fochteloerveen_Norgerholt2020</t>
-  </si>
-  <si>
-    <t>./DR Extra/NM_DCR2013/DCR2013_DigitaleStandaard/DCR fochteloo</t>
-  </si>
-  <si>
-    <t>./DR/NM_Westerbork2017/westerbork2017</t>
-  </si>
-  <si>
-    <t>./DR/SBB0817_Grolloerveen2013/0817_Hooghalen_Grolloo</t>
-  </si>
-  <si>
-    <t>./DR/SBB0863_Elperstroom_Schoonloo2012/0863_Elperstroom</t>
-  </si>
-  <si>
-    <t>./DR/SBB0936_DrentseAa2015_16/0936-DrentscheAa-vegetatiekartering 2015-2016</t>
-  </si>
-  <si>
-    <t>./FR/Bakkeveense_duinen/Fr 0752_Bakkefean_2009/752_Bakkefean</t>
-  </si>
-  <si>
-    <t>./FR/Bakkeveense_duinen/Slotplaats_2016/slotplaats</t>
-  </si>
-  <si>
-    <t>./FR/Duinen_Ameland/Ameland_2010/0808_Ameland</t>
-  </si>
-  <si>
-    <t>./FR/Duinen_Schiermonnikoog/Schiermonnikoog_2015/digitale standaard/Schiermonnikoog2015</t>
-  </si>
-  <si>
-    <t>./FR/Duinen_Schiermonnikoog/Schiermonnikoog_2017/DS_SchiermonnikoogProv_2017</t>
-  </si>
-  <si>
-    <t>./FR/Duinen_Terschelling/Terschelling_2012/0866-Terschelling</t>
-  </si>
-  <si>
-    <t>./FR/Lauwersmeer_Fryslan/Lauwersmeer_Fryslan_2015/933_VegKart_Lauwersmeer2015</t>
-  </si>
-  <si>
-    <t>./FR/Rottige_Meenthe_Brandemeer/Rottige_Meenthe_Brandemeer_2013/864_RottigeMeenthe2013</t>
-  </si>
-  <si>
-    <t>./FR/Sneekermeergebied/Vegetatiekartering 2009/Terkaplester puollen/761_vegKartTerkapPuollen_2009</t>
-  </si>
-  <si>
-    <t>./FR Extra/2022_Bakkefean/Database/DS_Bakkefean2022_NM_SBB</t>
-  </si>
-  <si>
-    <t>./FR Extra/FRP1-3 Snitsermar 2021_DIGITALE OPLEVERMAP definitief/digitale standaard/FRP1-3_Snitsermar_2021</t>
-  </si>
-  <si>
-    <t>./FR Extra/Fryslan -De Deelen e.o. 2022/digitale standaard/FRP1-3_De Deelen e.o._2022</t>
-  </si>
-  <si>
-    <t>./GR/SBB Duurswold2013/0813_Duurswold</t>
-  </si>
-  <si>
-    <t>./GR/SBB Westerwolde 2020/Database/Westerwolde2020</t>
-  </si>
-  <si>
-    <t>./GR/SGL Zuidlaardermeer 2019/kartering zuidlaardermeer 2019 definitief/Database Zuidlaardermeer 2019/DS_Zuidlaardermeer2019</t>
-  </si>
-  <si>
     <t>path_csvs</t>
   </si>
   <si>
@@ -294,66 +225,39 @@
     <t>./FR Extra/2022_Bakkefean/GISbestanden/vlakken.shp</t>
   </si>
   <si>
-    <t>./GR/SBB ZWK 2010/0815_Trimunt_2010/815_Trimunt</t>
-  </si>
-  <si>
-    <t>./GR/SBB Lauwersmeer 2015/933_VegKart_Lauwersmeer2015</t>
-  </si>
-  <si>
     <t>OBJECTID</t>
   </si>
   <si>
-    <t>./FR/Duinen_Vlieland/Vegetatiekartering 2013/890_Vlieland2013</t>
-  </si>
-  <si>
-    <t>./GR/NM vegetatiekartering RuitenAa2020/digi standaard_RuitenA_2020/digi standaard_RuitenA_2020</t>
-  </si>
-  <si>
     <t>./GR/NM vegetatiekartering RuitenAa2020/vegkart_RuitenA_2020/vegkart_RuitenA_2020.shp</t>
   </si>
   <si>
     <t>NM_Fochteloerveen2013_14</t>
   </si>
   <si>
-    <t>./DR/NM_Fochteloerveen2013_14/digitale standaard/Fochteloerveen2013-2014</t>
-  </si>
-  <si>
     <t>./DR/NM_Fochteloerveen2013_14/NM_Fochteloerveen2013_14.shp</t>
   </si>
   <si>
     <t>NM_Klencke2018</t>
   </si>
   <si>
-    <t>./DR/NM_Klencke2018/DS_DeKlencke_2018</t>
-  </si>
-  <si>
     <t>./DR/NM_Klencke2018/NM_deKlencke2018.shp</t>
   </si>
   <si>
     <t>NM_Leggelderveld2020</t>
   </si>
   <si>
-    <t>./DR/NM_Leggelderveld2020/Leggelderveld 2020</t>
-  </si>
-  <si>
     <t>./DR/NM_Leggelderveld2020/NM_Leggelderveld2020.shp</t>
   </si>
   <si>
     <t>SBB0756_Drentsche_A2009</t>
   </si>
   <si>
-    <t>./DR/SBB0756_Drentsche_A2009/756_Drentse_Aa</t>
-  </si>
-  <si>
     <t>./DR/SBB0756_Drentsche_A2009/SBB0756_DrentscheAa2009.shp</t>
   </si>
   <si>
     <t>SBB0757_De_Velden2009</t>
   </si>
   <si>
-    <t>./DR/SBB0757_De_Velden2009/De_Velden</t>
-  </si>
-  <si>
     <t>vlakken_EL</t>
   </si>
   <si>
@@ -363,36 +267,24 @@
     <t>SBB0763_Terhorst2009</t>
   </si>
   <si>
-    <t>./DR/SBB0763_Terhorst2009/763_Terhorst</t>
-  </si>
-  <si>
     <t>./DR/SBB0763_Terhorst2009/SBB0763_Terhorst2009.shp</t>
   </si>
   <si>
     <t>SBB0816_Norg2010</t>
   </si>
   <si>
-    <t>./DR/SBB0816_Norg2010/816_Norg</t>
-  </si>
-  <si>
     <t>./DR/SBB0816_Norg2010/SBB0816Norg2010.shp</t>
   </si>
   <si>
     <t>SBB0881_SBB_Ruinen_Havelterberg2013</t>
   </si>
   <si>
-    <t>./DR/SBB0881_SBB_Ruinen_Havelterberg2013/881_RuinenHavelte</t>
-  </si>
-  <si>
     <t>./DR/SBB0881_SBB_Ruinen_Havelterberg2013/SBB0881_Ruinen_Havelterberg2013.shp</t>
   </si>
   <si>
     <t>SBB0935_DrentsFrieseWold2015</t>
   </si>
   <si>
-    <t>./DR/SBB0935_DrentsFrieseWold2015/digitale standaard/935_VegKart_DrentsFrieseWold2015</t>
-  </si>
-  <si>
     <t>elmid</t>
   </si>
   <si>
@@ -402,109 +294,217 @@
     <t>SBB1034_Dwingelderveld2017</t>
   </si>
   <si>
-    <t>./DR/SBB1034_Dwingelderveld2017/1034-Database</t>
-  </si>
-  <si>
     <t>./DR/SBB1034_Dwingelderveld2017/SBB1034_Dwingelderveld2017.shp</t>
   </si>
   <si>
     <t>SBB1039_Drenthe2019</t>
   </si>
   <si>
-    <t>./DR/SBB1039_Drenthe2019/1039_Drenthe_2019</t>
-  </si>
-  <si>
     <t>./DR/SBB1039_Drenthe2019/SBB1039_Drenthe_2019_Arnoud.shp</t>
   </si>
   <si>
     <t>GL_Zuidlaardermeer2019</t>
   </si>
   <si>
-    <t>./DR/GL_Zuidlaardermeer2019/DS_Zuidlaardermeer2019</t>
-  </si>
-  <si>
     <t>./DR/GL_Zuidlaardermeer2019/GL_Zuidlaardermeer2019.shp</t>
   </si>
   <si>
     <t>NM_Mantingerveld2020</t>
   </si>
   <si>
-    <t>./DR/NM_Mantingerveld2020/Mantingerveld_digi standaard NMv3.01</t>
-  </si>
-  <si>
     <t>./DR/NM_Mantingerveld2020/NM_Mantingerveld2020.shp</t>
   </si>
   <si>
     <t>NM_Norg_heiden2020</t>
   </si>
   <si>
-    <t>./DR/NM_Norg_heiden2020/Norg_heide 2020</t>
-  </si>
-  <si>
     <t>./DR/NM_Norg_heiden2020/NM_Norg_heide2020.shp</t>
   </si>
   <si>
     <t>NM_NorgerBeekdal2018</t>
   </si>
   <si>
-    <t>./DR/NM_NorgerBeekdal2018/digi standaard vegkart NEL</t>
-  </si>
-  <si>
     <t>./DR/NM_NorgerBeekdal2018/NM_NorgerBeekdal2018.shp</t>
   </si>
   <si>
     <t>NM_SBB_Fochteloerveen_randen2016</t>
   </si>
   <si>
-    <t>./DR/NM_SBB_Fochteloerveen_randen2016/fochteloo2016</t>
-  </si>
-  <si>
     <t>./DR/NM_SBB_Fochteloerveen_randen2016/NM_SBB_Fochteloerveen_randen2016.shp</t>
   </si>
   <si>
     <t>Drouwenerzand_2020</t>
   </si>
   <si>
-    <t>./DR Extra/2020_Drouwenerzand/bron oplevering Drouwenerzand/Digitale_Standaard_Drouwenerzand2020</t>
-  </si>
-  <si>
     <t>./DR Extra/2020_Drouwenerzand/HDL_Drouwenerzand_2020.shp</t>
   </si>
   <si>
     <t>Sneekermeergebied_2009</t>
   </si>
   <si>
-    <t>./FR/Sneekermeergebied/Vegetatiekartering 2009/Snitsermar/760_vegkartSnitsermar2009</t>
-  </si>
-  <si>
     <t>./FR/Sneekermeergebied/Vegetatiekartering 2009/Snitsermar/vlakken.shp</t>
   </si>
   <si>
     <t>SBB ZWK 2010 0814_Tussen de Gasten 2010</t>
   </si>
   <si>
-    <t>./GR/SBB ZWK 2010/0814_Tussen de Gasten 2010/0814_Tussen de Gasten</t>
-  </si>
-  <si>
     <t>./GR/SBB ZWK 2010/0814_Tussen de Gasten 2010/ZWK0814_2010.shp</t>
   </si>
   <si>
     <t>SGL Hunzedal en Leekstermeer2021 Hunzedal</t>
   </si>
   <si>
-    <t>./GR/SGL Hunzedal en Leekstermeer2021/2021 Vegetatie- en plantensoortenkartering Hunzedal concept/digitale standaard/20-456_mdb</t>
-  </si>
-  <si>
     <t>./GR/SGL Hunzedal en Leekstermeer2021/2021 Vegetatie- en plantensoortenkartering Hunzedal concept/gis/Vegetatiekartering_Hunzedal2021.shp</t>
   </si>
   <si>
     <t>SGL Hunzedal en Leekstermeer2021 Leekstermeer 2021</t>
   </si>
   <si>
-    <t>./GR/SGL Hunzedal en Leekstermeer2021/2021 Vegetatiekartering Leekstermeer2021/Database Onlanden_2021/DS_Onlanden2021_v20-01-22</t>
-  </si>
-  <si>
     <t>./GR/SGL Hunzedal en Leekstermeer2021/2021 Vegetatiekartering Leekstermeer2021/GIS bestanden Onlanden 2021/Vegetatiekartering_Leekstermeer2021.shp</t>
+  </si>
+  <si>
+    <t>./DR Extra/NM_DCR2013/DCR2013_DigitaleStandaard/DCR fochteloo.mdb</t>
+  </si>
+  <si>
+    <t>./DR/NM_Westerbork2017/westerbork2017.mdb</t>
+  </si>
+  <si>
+    <t>./DR/SBB0817_Grolloerveen2013/0817_Hooghalen_Grolloo.mdb</t>
+  </si>
+  <si>
+    <t>./DR/SBB0863_Elperstroom_Schoonloo2012/0863_Elperstroom.mdb</t>
+  </si>
+  <si>
+    <t>./DR/SBB0936_DrentseAa2015_16/0936-DrentscheAa-vegetatiekartering 2015-2016.mdb</t>
+  </si>
+  <si>
+    <t>./FR/Bakkeveense_duinen/Fr 0752_Bakkefean_2009/752_Bakkefean.mdb</t>
+  </si>
+  <si>
+    <t>./FR/Bakkeveense_duinen/Slotplaats_2016/slotplaats.mdb</t>
+  </si>
+  <si>
+    <t>./FR/Duinen_Ameland/Ameland_2010/0808_Ameland.mdb</t>
+  </si>
+  <si>
+    <t>./FR/Duinen_Schiermonnikoog/Schiermonnikoog_2015/digitale standaard/Schiermonnikoog2015.mdb</t>
+  </si>
+  <si>
+    <t>./FR/Duinen_Schiermonnikoog/Schiermonnikoog_2017/DS_SchiermonnikoogProv_2017.mdb</t>
+  </si>
+  <si>
+    <t>./FR/Duinen_Terschelling/Terschelling_2012/0866-Terschelling.mdb</t>
+  </si>
+  <si>
+    <t>./FR/Duinen_Vlieland/Vegetatiekartering 2013/890_Vlieland2013.mdb</t>
+  </si>
+  <si>
+    <t>./FR/Lauwersmeer_Fryslan/Lauwersmeer_Fryslan_2015/933_VegKart_Lauwersmeer2015.mdb</t>
+  </si>
+  <si>
+    <t>./FR/Rottige_Meenthe_Brandemeer/Rottige_Meenthe_Brandemeer_2013/864_RottigeMeenthe2013.mdb</t>
+  </si>
+  <si>
+    <t>./FR/Sneekermeergebied/Vegetatiekartering 2009/Terkaplester puollen/761_vegKartTerkapPuollen_2009.mdb</t>
+  </si>
+  <si>
+    <t>./FR Extra/2022_Bakkefean/Database/DS_Bakkefean2022_NM_SBB.mdb</t>
+  </si>
+  <si>
+    <t>./FR Extra/FRP1-3 Snitsermar 2021_DIGITALE OPLEVERMAP definitief/digitale standaard/FRP1-3_Snitsermar_2021.mdb</t>
+  </si>
+  <si>
+    <t>./FR Extra/Fryslan -De Deelen e.o. 2022/digitale standaard/FRP1-3_De Deelen e.o._2022.mdb</t>
+  </si>
+  <si>
+    <t>./FR Extra/Tjonger_2021_SBB/Database/Tjonger_2021.mdb</t>
+  </si>
+  <si>
+    <t>./FR Extra/Witte en zwarte brekken Veg&amp;Flora 2021/turbovegDS/Wite_en_Swarte_Brekken_2021.mdb</t>
+  </si>
+  <si>
+    <t>./GR/NM vegetatiekartering RuitenAa2020/digi standaard_RuitenA_2020/digi standaard_RuitenA_2020.mdb</t>
+  </si>
+  <si>
+    <t>./GR/SBB Duurswold2013/0813_Duurswold.mdb</t>
+  </si>
+  <si>
+    <t>./GR/SBB Lauwersmeer 2015/933_VegKart_Lauwersmeer2015.mdb</t>
+  </si>
+  <si>
+    <t>./GR/SBB Westerwolde 2020/Database/Westerwolde2020.mdb</t>
+  </si>
+  <si>
+    <t>./GR/SBB ZWK 2010/0815_Trimunt_2010/815_Trimunt.mdb</t>
+  </si>
+  <si>
+    <t>./GR/SGL Zuidlaardermeer 2019/kartering zuidlaardermeer 2019 definitief/Database Zuidlaardermeer 2019/DS_Zuidlaardermeer2019.mdb</t>
+  </si>
+  <si>
+    <t>./DR/NM_Fochteloerveen2013_14/digitale standaard/Fochteloerveen2013-2014.mdb</t>
+  </si>
+  <si>
+    <t>./DR/NM_Klencke2018/DS_DeKlencke_2018.mdb</t>
+  </si>
+  <si>
+    <t>./DR/NM_Leggelderveld2020/Leggelderveld 2020.mdb</t>
+  </si>
+  <si>
+    <t>./DR/SBB0756_Drentsche_A2009/756_Drentse_Aa.mdb</t>
+  </si>
+  <si>
+    <t>./DR/SBB0757_De_Velden2009/De_Velden.mdb</t>
+  </si>
+  <si>
+    <t>./DR/SBB0763_Terhorst2009/763_Terhorst.mdb</t>
+  </si>
+  <si>
+    <t>./DR/SBB0816_Norg2010/816_Norg.mdb</t>
+  </si>
+  <si>
+    <t>./DR/SBB0881_SBB_Ruinen_Havelterberg2013/881_RuinenHavelte.mdb</t>
+  </si>
+  <si>
+    <t>./DR/SBB0935_DrentsFrieseWold2015/digitale standaard/935_VegKart_DrentsFrieseWold2015.mdb</t>
+  </si>
+  <si>
+    <t>./DR/SBB1034_Dwingelderveld2017/1034-Database.mdb</t>
+  </si>
+  <si>
+    <t>./DR/SBB1039_Drenthe2019/1039_Drenthe_2019.mdb</t>
+  </si>
+  <si>
+    <t>./DR/GL_Zuidlaardermeer2019/DS_Zuidlaardermeer2019.mdb</t>
+  </si>
+  <si>
+    <t>./DR/NM_Mantingerveld2020/Mantingerveld_digi standaard NMv3.01.mdb</t>
+  </si>
+  <si>
+    <t>./DR/NM_Norg_heiden2020/Norg_heide 2020.mdb</t>
+  </si>
+  <si>
+    <t>./DR/NM_NorgerBeekdal2018/digi standaard vegkart NEL.mdb</t>
+  </si>
+  <si>
+    <t>./DR/NM_SBB_Fochteloerveen_randen2016/fochteloo2016.mdb</t>
+  </si>
+  <si>
+    <t>./DR Extra/2020_Drouwenerzand/bron oplevering Drouwenerzand/Digitale_Standaard_Drouwenerzand2020.mdb</t>
+  </si>
+  <si>
+    <t>./FR/Sneekermeergebied/Vegetatiekartering 2009/Snitsermar/760_vegkartSnitsermar2009.mdb</t>
+  </si>
+  <si>
+    <t>./GR/SBB ZWK 2010/0814_Tussen de Gasten 2010/0814_Tussen de Gasten.mdb</t>
+  </si>
+  <si>
+    <t>./GR/SGL Hunzedal en Leekstermeer2021/2021 Vegetatiekartering Leekstermeer2021/Database Onlanden_2021/DS_Onlanden2021_v20-01-22.mdb</t>
+  </si>
+  <si>
+    <t>./DR Extra/definitief Fochteloo_Norg2020/GISbestanden_Fochteloo_Norg2020/VlakkenVegetatiekarteringFochteloo_210331/DS_NM_SBB v3.0Fochteloerveen_Norgerholt2020.mdb</t>
+  </si>
+  <si>
+    <t>./GR/SGL Hunzedal en Leekstermeer2021/2021 Vegetatie- en plantensoortenkartering Hunzedal concept/digitale standaard/20-456_VegKart_Onnerpolder2021.mdb</t>
   </si>
 </sst>
 </file>
@@ -863,14 +863,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="127.7109375" customWidth="1"/>
+    <col min="3" max="3" width="153.140625" customWidth="1"/>
     <col min="4" max="4" width="64" customWidth="1"/>
     <col min="5" max="5" width="131.140625" customWidth="1"/>
   </cols>
@@ -883,10 +883,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -907,10 +907,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>158</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -924,10 +924,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>112</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -941,10 +941,10 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>113</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -958,10 +958,10 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>114</v>
       </c>
       <c r="D5" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
@@ -975,10 +975,10 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
@@ -992,10 +992,10 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>116</v>
       </c>
       <c r="D7" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E7" t="s">
         <v>16</v>
@@ -1009,10 +1009,10 @@
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>117</v>
       </c>
       <c r="D8" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
         <v>19</v>
@@ -1026,10 +1026,10 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>118</v>
       </c>
       <c r="D9" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E9" t="s">
         <v>21</v>
@@ -1043,10 +1043,10 @@
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>119</v>
       </c>
       <c r="D10" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
         <v>23</v>
@@ -1060,10 +1060,10 @@
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="D11" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>
@@ -1077,10 +1077,10 @@
         <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>121</v>
       </c>
       <c r="D12" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
         <v>27</v>
@@ -1094,13 +1094,13 @@
         <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>122</v>
       </c>
       <c r="D13" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1111,10 +1111,10 @@
         <v>29</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>92</v>
+        <v>123</v>
       </c>
       <c r="D14" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E14" t="s">
         <v>30</v>
@@ -1128,10 +1128,10 @@
         <v>31</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>32</v>
@@ -1152,10 +1152,10 @@
         <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>125</v>
       </c>
       <c r="D16" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="E16" t="s">
         <v>34</v>
@@ -1169,10 +1169,10 @@
         <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>75</v>
+        <v>126</v>
       </c>
       <c r="D17" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="E17" t="s">
         <v>36</v>
@@ -1186,13 +1186,13 @@
         <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>76</v>
+        <v>127</v>
       </c>
       <c r="D18" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E18" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1203,10 +1203,10 @@
         <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>128</v>
       </c>
       <c r="D19" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="E19" t="s">
         <v>40</v>
@@ -1220,10 +1220,10 @@
         <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>129</v>
       </c>
       <c r="D20" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="E20" t="s">
         <v>42</v>
@@ -1237,10 +1237,10 @@
         <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>130</v>
       </c>
       <c r="D21" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="E21" t="s">
         <v>44</v>
@@ -1254,10 +1254,10 @@
         <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>131</v>
       </c>
       <c r="D22" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="E22" t="s">
         <v>46</v>
@@ -1271,13 +1271,13 @@
         <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="D23" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="E23" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="K23" s="3"/>
     </row>
@@ -1289,10 +1289,10 @@
         <v>49</v>
       </c>
       <c r="C24" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="D24" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="E24" t="s">
         <v>50</v>
@@ -1306,10 +1306,10 @@
         <v>51</v>
       </c>
       <c r="C25" t="s">
-        <v>90</v>
+        <v>134</v>
       </c>
       <c r="D25" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="E25" t="s">
         <v>52</v>
@@ -1324,10 +1324,10 @@
         <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>135</v>
       </c>
       <c r="D26" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E26" t="s">
         <v>54</v>
@@ -1341,10 +1341,10 @@
         <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>89</v>
+        <v>136</v>
       </c>
       <c r="D27" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="E27" t="s">
         <v>56</v>
@@ -1358,10 +1358,10 @@
         <v>57</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>81</v>
+        <v>137</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>58</v>
@@ -1379,16 +1379,16 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="D29" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="E29" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -1396,16 +1396,16 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>99</v>
+        <v>139</v>
       </c>
       <c r="D30" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E30" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -1413,16 +1413,16 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="D31" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E31" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -1430,16 +1430,16 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>105</v>
+        <v>141</v>
       </c>
       <c r="D32" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E32" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1447,16 +1447,16 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>108</v>
+        <v>142</v>
       </c>
       <c r="D33" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="E33" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1464,16 +1464,16 @@
         <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="D34" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="E34" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1481,16 +1481,16 @@
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>115</v>
+        <v>144</v>
       </c>
       <c r="D35" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="E35" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1498,16 +1498,16 @@
         <v>8</v>
       </c>
       <c r="B36" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>118</v>
+        <v>145</v>
       </c>
       <c r="D36" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="E36" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1515,16 +1515,16 @@
         <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="D37" t="s">
-        <v>122</v>
+        <v>86</v>
       </c>
       <c r="E37" t="s">
-        <v>123</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1532,16 +1532,16 @@
         <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>124</v>
+        <v>88</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="D38" t="s">
-        <v>122</v>
+        <v>86</v>
       </c>
       <c r="E38" t="s">
-        <v>126</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1549,16 +1549,16 @@
         <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>127</v>
+        <v>90</v>
       </c>
       <c r="C39" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="D39" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E39" t="s">
-        <v>129</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1566,16 +1566,16 @@
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>130</v>
+        <v>92</v>
       </c>
       <c r="C40" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="D40" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="E40" t="s">
-        <v>132</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1583,16 +1583,16 @@
         <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>133</v>
+        <v>94</v>
       </c>
       <c r="C41" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="D41" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E41" t="s">
-        <v>135</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1600,16 +1600,16 @@
         <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
       <c r="C42" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="D42" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E42" t="s">
-        <v>138</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1617,16 +1617,16 @@
         <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>139</v>
+        <v>98</v>
       </c>
       <c r="C43" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="D43" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E43" t="s">
-        <v>141</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1634,16 +1634,16 @@
         <v>8</v>
       </c>
       <c r="B44" t="s">
-        <v>142</v>
+        <v>100</v>
       </c>
       <c r="C44" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="D44" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E44" t="s">
-        <v>144</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1651,16 +1651,16 @@
         <v>8</v>
       </c>
       <c r="B45" t="s">
-        <v>145</v>
+        <v>102</v>
       </c>
       <c r="C45" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D45" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="E45" t="s">
-        <v>147</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1668,16 +1668,16 @@
         <v>17</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>148</v>
+        <v>104</v>
       </c>
       <c r="C46" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="D46" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="E46" t="s">
-        <v>150</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1685,16 +1685,16 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>151</v>
+        <v>106</v>
       </c>
       <c r="C47" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D47" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="E47" t="s">
-        <v>153</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1702,16 +1702,16 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>154</v>
+        <v>108</v>
       </c>
       <c r="C48" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D48" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="E48" t="s">
-        <v>156</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1719,16 +1719,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
+        <v>110</v>
+      </c>
+      <c r="C49" t="s">
         <v>157</v>
       </c>
-      <c r="C49" t="s">
-        <v>158</v>
-      </c>
       <c r="D49" t="s">
-        <v>122</v>
+        <v>86</v>
       </c>
       <c r="E49" t="s">
-        <v>159</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>